<commit_message>
v3 stable, mais pas très efficace
</commit_message>
<xml_diff>
--- a/doc/Etudes.xlsx
+++ b/doc/Etudes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halte\reposDivers\LeSolitaire\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halte\reposDivers\LeSolitaireV2\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BAE438-37BB-4E1E-917B-990B406A8E36}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D484CA-B9A9-4FB3-86E8-833BA0E27D48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{EDDB1EC0-7760-4179-9333-21B76CBF73A8}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{EDDB1EC0-7760-4179-9333-21B76CBF73A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Les 1ières situations" sheetId="1" r:id="rId1"/>
@@ -569,7 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E3F4F2-A6E5-4649-95B9-CA21165F464E}">
   <dimension ref="A1:BE90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection sqref="A1:AI1"/>
     </sheetView>
   </sheetViews>
@@ -5297,7 +5297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845A97F2-01A0-48A0-AF97-CF14E0D68EE2}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
OK : Initialisation, gestion ED, EF
</commit_message>
<xml_diff>
--- a/doc/Etudes.xlsx
+++ b/doc/Etudes.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halte\reposDivers\LeSolitaireV2\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halte\reposDivers\LeSolitaire\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D484CA-B9A9-4FB3-86E8-833BA0E27D48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CEF749-FCD1-42C6-A46C-4160BAD67497}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{EDDB1EC0-7760-4179-9333-21B76CBF73A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{EDDB1EC0-7760-4179-9333-21B76CBF73A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Les 1ières situations" sheetId="1" r:id="rId1"/>
     <sheet name="Coordonnées" sheetId="2" r:id="rId2"/>
+    <sheet name="Dualité" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="exposant">'Les 1ières situations'!#REF!</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="19">
   <si>
     <t>x</t>
   </si>
@@ -57,6 +58,48 @@
   </si>
   <si>
     <t>Autres situations obtenues après un mouvement depuis une des 8 situations initiales originales, mais ayant un équivalent par symétrie ci-dessus.</t>
+  </si>
+  <si>
+    <t>On obtient</t>
+  </si>
+  <si>
+    <t>(-2,-2),(-1,-2) -&gt; (0,-2)</t>
+  </si>
+  <si>
+    <t>(0,-2),(0,-1)-&gt; (0,0)</t>
+  </si>
+  <si>
+    <t>A partir de cette situation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jouons les mouvements DIRECTS suivants </t>
+  </si>
+  <si>
+    <t>A partir de cette situation DUALE de la situation finale</t>
+  </si>
+  <si>
+    <t>Jouons les mouvements dans l'ordre inverse</t>
+  </si>
+  <si>
+    <t>Si la situation initiale n'a qu'une case vide, la situation duale est gagnante.</t>
+  </si>
+  <si>
+    <t>Evidemment, on ne peut pas avoir égalité d'une situation avec sa duale.</t>
+  </si>
+  <si>
+    <t>Mais on peut s'interroger dans le cas où il y aurait égalité à une symétrie près.</t>
+  </si>
+  <si>
+    <t>Le jeu de mouvements serait le même à une symétrie près.</t>
+  </si>
+  <si>
+    <t>Hélas dans notre cas, ce n'est pas possible. La case centrale est toujours différente de sa duale, quelle que soit la symétrie envisagée.</t>
+  </si>
+  <si>
+    <t>On obtient la duale de la situation initiale</t>
+  </si>
+  <si>
+    <t>Donc si on arrive à une situation qui soit égale à sa duale, il suffit de rejouer les mouvements dans le sens inverse pour obtenir la duale de la situation initiale.</t>
   </si>
 </sst>
 </file>
@@ -189,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -252,6 +295,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5297,7 +5352,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845A97F2-01A0-48A0-AF97-CF14E0D68EE2}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5520,4 +5577,1095 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{812941E1-6BDF-491E-AA64-34D616D3FB05}">
+  <dimension ref="A1:R39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="8" width="4.28515625" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" customWidth="1"/>
+    <col min="11" max="17" width="4.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="26" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+    </row>
+    <row r="2" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1">
+        <v>-3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1">
+        <v>-3</v>
+      </c>
+      <c r="L2" s="1">
+        <v>-2</v>
+      </c>
+      <c r="M2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>-3</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="J3" s="4">
+        <v>-3</v>
+      </c>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+    </row>
+    <row r="4" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>-2</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="J4" s="4">
+        <v>-2</v>
+      </c>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="20"/>
+    </row>
+    <row r="5" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>-1</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>-1</v>
+      </c>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+    </row>
+    <row r="6" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>0</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+    </row>
+    <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+    </row>
+    <row r="8" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>2</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="20"/>
+      <c r="J8" s="4">
+        <v>2</v>
+      </c>
+      <c r="K8" s="20"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="20"/>
+    </row>
+    <row r="9" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>3</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="J9" s="4">
+        <v>3</v>
+      </c>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+    </row>
+    <row r="11" spans="1:18" s="26" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+    </row>
+    <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+    </row>
+    <row r="15" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1">
+        <v>-3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1">
+        <v>3</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1">
+        <v>-3</v>
+      </c>
+      <c r="L15" s="1">
+        <v>-2</v>
+      </c>
+      <c r="M15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <v>1</v>
+      </c>
+      <c r="P15" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>-3</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="J16" s="4">
+        <v>-3</v>
+      </c>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+    </row>
+    <row r="17" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>-2</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="20"/>
+      <c r="J17" s="4">
+        <v>-2</v>
+      </c>
+      <c r="K17" s="20"/>
+      <c r="L17" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="20"/>
+    </row>
+    <row r="18" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>-1</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>-1</v>
+      </c>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+    </row>
+    <row r="19" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>0</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+    </row>
+    <row r="20" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>1</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1</v>
+      </c>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+    </row>
+    <row r="21" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>2</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="20"/>
+      <c r="J21" s="4">
+        <v>2</v>
+      </c>
+      <c r="K21" s="20"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="20"/>
+    </row>
+    <row r="22" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>3</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="J22" s="4">
+        <v>3</v>
+      </c>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+    </row>
+    <row r="24" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1">
+        <v>-3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>-2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1">
+        <v>-3</v>
+      </c>
+      <c r="L24" s="1">
+        <v>-2</v>
+      </c>
+      <c r="M24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0</v>
+      </c>
+      <c r="O24" s="1">
+        <v>1</v>
+      </c>
+      <c r="P24" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>-3</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="J25" s="4">
+        <v>-3</v>
+      </c>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+    </row>
+    <row r="26" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>-2</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="20"/>
+      <c r="J26" s="4">
+        <v>-2</v>
+      </c>
+      <c r="K26" s="20"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="20"/>
+    </row>
+    <row r="27" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>-1</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4">
+        <v>-1</v>
+      </c>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+    </row>
+    <row r="28" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>0</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J28" s="4">
+        <v>0</v>
+      </c>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+    </row>
+    <row r="29" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>1</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4">
+        <v>1</v>
+      </c>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+    </row>
+    <row r="30" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>2</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="20"/>
+      <c r="J30" s="4">
+        <v>2</v>
+      </c>
+      <c r="K30" s="20"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="20"/>
+    </row>
+    <row r="31" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>3</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="J31" s="4">
+        <v>3</v>
+      </c>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+    </row>
+    <row r="33" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23"/>
+    </row>
+    <row r="34" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="23"/>
+    </row>
+    <row r="35" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
+    </row>
+    <row r="36" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="23"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="23"/>
+      <c r="P36" s="23"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="23"/>
+    </row>
+    <row r="37" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="23"/>
+      <c r="P37" s="23"/>
+      <c r="Q37" s="23"/>
+      <c r="R37" s="23"/>
+    </row>
+    <row r="38" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23"/>
+      <c r="O38" s="23"/>
+      <c r="P38" s="23"/>
+      <c r="Q38" s="23"/>
+      <c r="R38" s="23"/>
+    </row>
+    <row r="39" spans="1:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="23"/>
+      <c r="P39" s="23"/>
+      <c r="Q39" s="23"/>
+      <c r="R39" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="J33:R33"/>
+    <mergeCell ref="A34:R34"/>
+    <mergeCell ref="A35:R35"/>
+    <mergeCell ref="A36:R36"/>
+    <mergeCell ref="A37:R37"/>
+    <mergeCell ref="A38:R38"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A39:R39"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="J14:R14"/>
+    <mergeCell ref="J1:R1"/>
+    <mergeCell ref="J11:R11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
B-Tree Persistant et Volatile, renommages et refactorisations
</commit_message>
<xml_diff>
--- a/doc/Etudes.xlsx
+++ b/doc/Etudes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhal2009\repos\Divers\LeSolitaire\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73387BA7-125D-437B-A6D0-C2947FA821E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1285098-0522-4617-A42D-DDE151726612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="696" activeTab="7" xr2:uid="{EDDB1EC0-7760-4179-9333-21B76CBF73A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="696" activeTab="8" xr2:uid="{EDDB1EC0-7760-4179-9333-21B76CBF73A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Les 1ères situations" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,8 @@
     <sheet name="EF en mémoire" sheetId="9" r:id="rId6"/>
     <sheet name="Dichotomie EF.dat" sheetId="7" r:id="rId7"/>
     <sheet name="saturé - minimal" sheetId="12" r:id="rId8"/>
+    <sheet name="Classique" sheetId="13" r:id="rId9"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId9"/>
-  </externalReferences>
   <definedNames>
     <definedName name="NbPierres">#REF!</definedName>
     <definedName name="ordre" localSheetId="7">'saturé - minimal'!$M$3</definedName>
@@ -52,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="69">
   <si>
     <t>x</t>
   </si>
@@ -233,17 +231,46 @@
   <si>
     <t>mini/maxi</t>
   </si>
+  <si>
+    <t>log(taille)</t>
+  </si>
+  <si>
+    <t>log(durée)</t>
+  </si>
+  <si>
+    <t>durée</t>
+  </si>
+  <si>
+    <t>log(nb)</t>
+  </si>
+  <si>
+    <t>Niveau</t>
+  </si>
+  <si>
+    <t>Statistiques d'exécution de la recherche en profondeur sur le plateau classique</t>
+  </si>
+  <si>
+    <t>nb elt</t>
+  </si>
+  <si>
+    <t>taille (octet)</t>
+  </si>
+  <si>
+    <t>durée (ms)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="d\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="171" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,6 +318,14 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -357,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -432,6 +467,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thick">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thick">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thick">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thick">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -439,7 +511,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -559,6 +631,8 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -595,6 +669,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Milliers" xfId="3" builtinId="3"/>
@@ -7277,6 +7363,1202 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Classique!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>log(nb)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Classique!$A$3:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Classique!$E$3:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.90308998699194354</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3802112417116059</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0374264979406238</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7176705030022621</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3745650607227651</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0096208408143248</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6071117413219582</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.1632806702619058</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.6740091618666817</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.1344636728794777</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.5404997799507534</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.8881889325574086</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.1734453104670832</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.3927776155288747</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B75-4158-B680-F009E4BFBE6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="763446376"/>
+        <c:axId val="763441128"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="763446376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="763441128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="763441128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="763446376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Classique!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>log(durée)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Classique!$A$3:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Classique!$F$3:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1.4771212547196624</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3424226808222062</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4623979978989561</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4771212547196624</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7634279935629373</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.12057393120585</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.705007959333336</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.3165993020938607</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8334658601706924</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.3495494835866353</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.7776225370647989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.19614577506825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.4752613928925244</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.7289946036631063</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C72B-4413-AD1D-323953FA0CCF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="772078952"/>
+        <c:axId val="772081904"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="772078952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="772081904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="772081904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="772078952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Classique!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>log(taille)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Classique!$A$3:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Classique!$G$3:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2.271841606536499</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.271841606536499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0969100130080562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6642658001476751</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3550106800911461</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9780709019742115</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5755434511631385</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.1338874813693645</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.6466447270916555</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.1074666364714068</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.5132605611240919</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.861441645926071</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.1475400363965864</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.3683878006101704</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2FBF-4BA7-91EF-53C1601432E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="532201888"/>
+        <c:axId val="532194344"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="532201888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532194344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="532194344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532201888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7358,6 +8640,126 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -8945,6 +10347,1554 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -9070,17 +12020,117 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Feuil1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Graphique 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5808911B-6AA1-495B-AC5F-571BF66970CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Graphique 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64C37FB5-8BB1-4F14-90A3-B41E45269A9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Graphique 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD19A19B-B95A-4D7D-B2F6-860B4FEA3360}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9411,43 +12461,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="53"/>
+      <c r="AF1" s="53"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="53"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
@@ -10118,50 +13168,50 @@
       <c r="AI9" s="2"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="53" t="s">
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="53"/>
-      <c r="S10" s="53" t="s">
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="55"/>
+      <c r="R10" s="55"/>
+      <c r="S10" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="T10" s="53"/>
-      <c r="U10" s="53"/>
-      <c r="V10" s="53"/>
-      <c r="W10" s="53"/>
-      <c r="X10" s="53"/>
-      <c r="Y10" s="53"/>
-      <c r="Z10" s="53"/>
-      <c r="AA10" s="53"/>
-      <c r="AB10" s="53" t="s">
+      <c r="T10" s="55"/>
+      <c r="U10" s="55"/>
+      <c r="V10" s="55"/>
+      <c r="W10" s="55"/>
+      <c r="X10" s="55"/>
+      <c r="Y10" s="55"/>
+      <c r="Z10" s="55"/>
+      <c r="AA10" s="55"/>
+      <c r="AB10" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="AC10" s="53"/>
-      <c r="AD10" s="53"/>
-      <c r="AE10" s="53"/>
-      <c r="AF10" s="53"/>
-      <c r="AG10" s="53"/>
-      <c r="AH10" s="53"/>
-      <c r="AI10" s="53"/>
-      <c r="AJ10" s="53"/>
+      <c r="AC10" s="55"/>
+      <c r="AD10" s="55"/>
+      <c r="AE10" s="55"/>
+      <c r="AF10" s="55"/>
+      <c r="AG10" s="55"/>
+      <c r="AH10" s="55"/>
+      <c r="AI10" s="55"/>
+      <c r="AJ10" s="55"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
@@ -10832,50 +13882,50 @@
       <c r="AI18" s="2"/>
     </row>
     <row r="19" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="53" t="s">
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="53"/>
-      <c r="P19" s="53"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="52" t="s">
+      <c r="K19" s="55"/>
+      <c r="L19" s="55"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="55"/>
+      <c r="S19" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="T19" s="52"/>
-      <c r="U19" s="52"/>
-      <c r="V19" s="52"/>
-      <c r="W19" s="52"/>
-      <c r="X19" s="52"/>
-      <c r="Y19" s="52"/>
-      <c r="Z19" s="52"/>
-      <c r="AA19" s="52"/>
-      <c r="AB19" s="53" t="s">
+      <c r="T19" s="54"/>
+      <c r="U19" s="54"/>
+      <c r="V19" s="54"/>
+      <c r="W19" s="54"/>
+      <c r="X19" s="54"/>
+      <c r="Y19" s="54"/>
+      <c r="Z19" s="54"/>
+      <c r="AA19" s="54"/>
+      <c r="AB19" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="AC19" s="53"/>
-      <c r="AD19" s="53"/>
-      <c r="AE19" s="53"/>
-      <c r="AF19" s="53"/>
-      <c r="AG19" s="53"/>
-      <c r="AH19" s="53"/>
-      <c r="AI19" s="53"/>
-      <c r="AJ19" s="53"/>
+      <c r="AC19" s="55"/>
+      <c r="AD19" s="55"/>
+      <c r="AE19" s="55"/>
+      <c r="AF19" s="55"/>
+      <c r="AG19" s="55"/>
+      <c r="AH19" s="55"/>
+      <c r="AI19" s="55"/>
+      <c r="AJ19" s="55"/>
     </row>
     <row r="20" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
@@ -10915,43 +13965,43 @@
       <c r="AI20" s="14"/>
     </row>
     <row r="21" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="51"/>
-      <c r="P21" s="51"/>
-      <c r="Q21" s="51"/>
-      <c r="R21" s="51"/>
-      <c r="S21" s="51"/>
-      <c r="T21" s="51"/>
-      <c r="U21" s="51"/>
-      <c r="V21" s="51"/>
-      <c r="W21" s="51"/>
-      <c r="X21" s="51"/>
-      <c r="Y21" s="51"/>
-      <c r="Z21" s="51"/>
-      <c r="AA21" s="51"/>
-      <c r="AB21" s="51"/>
-      <c r="AC21" s="51"/>
-      <c r="AD21" s="51"/>
-      <c r="AE21" s="51"/>
-      <c r="AF21" s="51"/>
-      <c r="AG21" s="51"/>
-      <c r="AH21" s="51"/>
-      <c r="AI21" s="51"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
+      <c r="N21" s="53"/>
+      <c r="O21" s="53"/>
+      <c r="P21" s="53"/>
+      <c r="Q21" s="53"/>
+      <c r="R21" s="53"/>
+      <c r="S21" s="53"/>
+      <c r="T21" s="53"/>
+      <c r="U21" s="53"/>
+      <c r="V21" s="53"/>
+      <c r="W21" s="53"/>
+      <c r="X21" s="53"/>
+      <c r="Y21" s="53"/>
+      <c r="Z21" s="53"/>
+      <c r="AA21" s="53"/>
+      <c r="AB21" s="53"/>
+      <c r="AC21" s="53"/>
+      <c r="AD21" s="53"/>
+      <c r="AE21" s="53"/>
+      <c r="AF21" s="53"/>
+      <c r="AG21" s="53"/>
+      <c r="AH21" s="53"/>
+      <c r="AI21" s="53"/>
       <c r="AL21"/>
       <c r="AM21"/>
       <c r="AN21"/>
@@ -12455,43 +15505,43 @@
       <c r="AR38" s="2"/>
     </row>
     <row r="40" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A40" s="51" t="s">
+      <c r="A40" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="51"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="51"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="51"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="51"/>
-      <c r="O40" s="51"/>
-      <c r="P40" s="51"/>
-      <c r="Q40" s="51"/>
-      <c r="R40" s="51"/>
-      <c r="S40" s="51"/>
-      <c r="T40" s="51"/>
-      <c r="U40" s="51"/>
-      <c r="V40" s="51"/>
-      <c r="W40" s="51"/>
-      <c r="X40" s="51"/>
-      <c r="Y40" s="51"/>
-      <c r="Z40" s="51"/>
-      <c r="AA40" s="51"/>
-      <c r="AB40" s="51"/>
-      <c r="AC40" s="51"/>
-      <c r="AD40" s="51"/>
-      <c r="AE40" s="51"/>
-      <c r="AF40" s="51"/>
-      <c r="AG40" s="51"/>
-      <c r="AH40" s="51"/>
-      <c r="AI40" s="51"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="53"/>
+      <c r="O40" s="53"/>
+      <c r="P40" s="53"/>
+      <c r="Q40" s="53"/>
+      <c r="R40" s="53"/>
+      <c r="S40" s="53"/>
+      <c r="T40" s="53"/>
+      <c r="U40" s="53"/>
+      <c r="V40" s="53"/>
+      <c r="W40" s="53"/>
+      <c r="X40" s="53"/>
+      <c r="Y40" s="53"/>
+      <c r="Z40" s="53"/>
+      <c r="AA40" s="53"/>
+      <c r="AB40" s="53"/>
+      <c r="AC40" s="53"/>
+      <c r="AD40" s="53"/>
+      <c r="AE40" s="53"/>
+      <c r="AF40" s="53"/>
+      <c r="AG40" s="53"/>
+      <c r="AH40" s="53"/>
+      <c r="AI40" s="53"/>
     </row>
     <row r="41" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
@@ -14684,30 +17734,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="43.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
       <c r="I2" s="28" t="s">
         <v>29</v>
       </c>
@@ -14971,16 +18021,16 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
       <c r="I16" s="24">
         <v>12524223</v>
       </c>
@@ -14994,31 +18044,31 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
       <c r="I19" s="28" t="s">
         <v>29</v>
       </c>
@@ -15157,16 +18207,16 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
       <c r="I26" s="24">
         <f>SUM(I21:I25)</f>
         <v>6147179</v>
@@ -15202,28 +18252,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="22" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="59" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
     </row>
     <row r="2" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -15504,28 +18554,28 @@
       <c r="Q9" s="20"/>
     </row>
     <row r="11" spans="1:18" s="22" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59" t="s">
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="59"/>
-      <c r="O11" s="59"/>
-      <c r="P11" s="59"/>
-      <c r="Q11" s="59"/>
-      <c r="R11" s="59"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="61"/>
+      <c r="O11" s="61"/>
+      <c r="P11" s="61"/>
+      <c r="Q11" s="61"/>
+      <c r="R11" s="61"/>
     </row>
     <row r="12" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -15544,28 +18594,28 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
+      <c r="A14" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60" t="s">
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="60"/>
-      <c r="R14" s="60"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="62"/>
+      <c r="O14" s="62"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="62"/>
     </row>
     <row r="15" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -16112,149 +19162,149 @@
       <c r="Q31" s="20"/>
     </row>
     <row r="33" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J33" s="58" t="s">
+      <c r="J33" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="58"/>
-      <c r="Q33" s="58"/>
-      <c r="R33" s="58"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="60"/>
     </row>
     <row r="34" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="58" t="s">
+      <c r="A34" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="58"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="58"/>
-      <c r="R34" s="58"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="60"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="60"/>
+      <c r="P34" s="60"/>
+      <c r="Q34" s="60"/>
+      <c r="R34" s="60"/>
     </row>
     <row r="35" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="58"/>
-      <c r="O35" s="58"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="58"/>
-      <c r="R35" s="58"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="60"/>
+      <c r="L35" s="60"/>
+      <c r="M35" s="60"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="60"/>
     </row>
     <row r="36" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="58" t="s">
+      <c r="A36" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="58"/>
-      <c r="K36" s="58"/>
-      <c r="L36" s="58"/>
-      <c r="M36" s="58"/>
-      <c r="N36" s="58"/>
-      <c r="O36" s="58"/>
-      <c r="P36" s="58"/>
-      <c r="Q36" s="58"/>
-      <c r="R36" s="58"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="60"/>
+      <c r="J36" s="60"/>
+      <c r="K36" s="60"/>
+      <c r="L36" s="60"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="60"/>
     </row>
     <row r="37" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="58" t="s">
+      <c r="A37" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="58"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="58"/>
-      <c r="K37" s="58"/>
-      <c r="L37" s="58"/>
-      <c r="M37" s="58"/>
-      <c r="N37" s="58"/>
-      <c r="O37" s="58"/>
-      <c r="P37" s="58"/>
-      <c r="Q37" s="58"/>
-      <c r="R37" s="58"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="60"/>
+      <c r="J37" s="60"/>
+      <c r="K37" s="60"/>
+      <c r="L37" s="60"/>
+      <c r="M37" s="60"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="60"/>
+      <c r="P37" s="60"/>
+      <c r="Q37" s="60"/>
+      <c r="R37" s="60"/>
     </row>
     <row r="38" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
-      <c r="J38" s="58"/>
-      <c r="K38" s="58"/>
-      <c r="L38" s="58"/>
-      <c r="M38" s="58"/>
-      <c r="N38" s="58"/>
-      <c r="O38" s="58"/>
-      <c r="P38" s="58"/>
-      <c r="Q38" s="58"/>
-      <c r="R38" s="58"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="60"/>
+      <c r="P38" s="60"/>
+      <c r="Q38" s="60"/>
+      <c r="R38" s="60"/>
     </row>
     <row r="39" spans="1:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="58" t="s">
+      <c r="A39" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="58"/>
-      <c r="C39" s="58"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="58"/>
-      <c r="F39" s="58"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="58"/>
-      <c r="J39" s="58"/>
-      <c r="K39" s="58"/>
-      <c r="L39" s="58"/>
-      <c r="M39" s="58"/>
-      <c r="N39" s="58"/>
-      <c r="O39" s="58"/>
-      <c r="P39" s="58"/>
-      <c r="Q39" s="58"/>
-      <c r="R39" s="58"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="60"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="60"/>
+      <c r="H39" s="60"/>
+      <c r="I39" s="60"/>
+      <c r="J39" s="60"/>
+      <c r="K39" s="60"/>
+      <c r="L39" s="60"/>
+      <c r="M39" s="60"/>
+      <c r="N39" s="60"/>
+      <c r="O39" s="60"/>
+      <c r="P39" s="60"/>
+      <c r="Q39" s="60"/>
+      <c r="R39" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -16299,16 +19349,16 @@
       <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -16325,17 +19375,17 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="K3" s="53" t="s">
+      <c r="K3" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="T3" s="61" t="s">
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="T3" s="63" t="s">
         <v>36</v>
       </c>
       <c r="U3" s="4">
@@ -16422,7 +19472,7 @@
       <c r="R4" s="1">
         <v>3</v>
       </c>
-      <c r="T4" s="61"/>
+      <c r="T4" s="63"/>
       <c r="U4" s="4">
         <v>-1</v>
       </c>
@@ -16703,17 +19753,17 @@
       <c r="B13">
         <v>0</v>
       </c>
-      <c r="K13" s="53" t="s">
+      <c r="K13" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="L13" s="53"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="53"/>
-      <c r="P13" s="53"/>
-      <c r="Q13" s="53"/>
-      <c r="R13" s="53"/>
-      <c r="T13" s="62" t="s">
+      <c r="L13" s="55"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="55"/>
+      <c r="Q13" s="55"/>
+      <c r="R13" s="55"/>
+      <c r="T13" s="64" t="s">
         <v>36</v>
       </c>
       <c r="U13" s="1">
@@ -16808,7 +19858,7 @@
       <c r="R14" s="1">
         <v>3</v>
       </c>
-      <c r="T14" s="62"/>
+      <c r="T14" s="64"/>
       <c r="U14" s="1">
         <v>-3</v>
       </c>
@@ -17082,8 +20132,8 @@
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="X26" s="53"/>
-      <c r="Y26" s="53"/>
+      <c r="X26" s="55"/>
+      <c r="Y26" s="55"/>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -26464,7 +29514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06B17AF-5054-4E2D-ACD8-E4A325ED7828}">
   <dimension ref="A1:U106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
@@ -26546,7 +29596,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="49">
-        <f t="dataTable" ref="C6:J36" dt2D="1" dtr="1" r1="M2" r2="M3" ca="1"/>
+        <f t="dataTable" ref="C6:J36" dt2D="1" dtr="1" r1="M2" r2="M3"/>
         <v>1</v>
       </c>
       <c r="D6" s="49">
@@ -27564,7 +30614,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="50">
-        <f t="dataTable" ref="C41:J71" dt2D="1" dtr="1" r1="M2" r2="M3"/>
+        <f t="dataTable" ref="C41:J71" dt2D="1" dtr="1" r1="M2" r2="M3" ca="1"/>
         <v>1</v>
       </c>
       <c r="D41" s="50">
@@ -29652,6 +32702,556 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A525DC-779D-4A1F-889C-06F99BC0B4C3}">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="52" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="67"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="52" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="70">
+        <v>8</v>
+      </c>
+      <c r="C3" s="52">
+        <v>30</v>
+      </c>
+      <c r="D3" s="52">
+        <v>187</v>
+      </c>
+      <c r="E3" s="68">
+        <f>LOG10(B3)</f>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="F3" s="68">
+        <f t="shared" ref="F3:G3" si="0">LOG10(C3)</f>
+        <v>1.4771212547196624</v>
+      </c>
+      <c r="G3" s="68">
+        <f t="shared" si="0"/>
+        <v>2.271841606536499</v>
+      </c>
+      <c r="H3" s="69">
+        <f>C3/24/60/60/1000</f>
+        <v>3.4722222222222219E-7</v>
+      </c>
+      <c r="J3" s="70">
+        <f>10^(0.5*A3+0.65)</f>
+        <v>14.125375446227544</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="70">
+        <v>24</v>
+      </c>
+      <c r="C4" s="52">
+        <v>22</v>
+      </c>
+      <c r="D4" s="52">
+        <v>187</v>
+      </c>
+      <c r="E4" s="68">
+        <f t="shared" ref="E4:E16" si="1">LOG10(B4)</f>
+        <v>1.3802112417116059</v>
+      </c>
+      <c r="F4" s="68">
+        <f t="shared" ref="F4:F16" si="2">LOG10(C4)</f>
+        <v>1.3424226808222062</v>
+      </c>
+      <c r="G4" s="68">
+        <f t="shared" ref="G4:G16" si="3">LOG10(D4)</f>
+        <v>2.271841606536499</v>
+      </c>
+      <c r="H4" s="69">
+        <f t="shared" ref="H4:H16" si="4">C4/24/60/60/1000</f>
+        <v>2.5462962962962958E-7</v>
+      </c>
+      <c r="J4" s="70">
+        <f t="shared" ref="J4:J16" si="5">10^(0.5*A4+0.65)</f>
+        <v>44.668359215096324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="70">
+        <v>109</v>
+      </c>
+      <c r="C5" s="52">
+        <v>29</v>
+      </c>
+      <c r="D5" s="52">
+        <v>1250</v>
+      </c>
+      <c r="E5" s="68">
+        <f t="shared" si="1"/>
+        <v>2.0374264979406238</v>
+      </c>
+      <c r="F5" s="68">
+        <f t="shared" si="2"/>
+        <v>1.4623979978989561</v>
+      </c>
+      <c r="G5" s="68">
+        <f t="shared" si="3"/>
+        <v>3.0969100130080562</v>
+      </c>
+      <c r="H5" s="69">
+        <f t="shared" si="4"/>
+        <v>3.356481481481481E-7</v>
+      </c>
+      <c r="J5" s="70">
+        <f t="shared" si="5"/>
+        <v>141.25375446227542</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="70">
+        <v>522</v>
+      </c>
+      <c r="C6" s="52">
+        <v>30</v>
+      </c>
+      <c r="D6" s="52">
+        <v>4616</v>
+      </c>
+      <c r="E6" s="68">
+        <f t="shared" si="1"/>
+        <v>2.7176705030022621</v>
+      </c>
+      <c r="F6" s="68">
+        <f t="shared" si="2"/>
+        <v>1.4771212547196624</v>
+      </c>
+      <c r="G6" s="68">
+        <f t="shared" si="3"/>
+        <v>3.6642658001476751</v>
+      </c>
+      <c r="H6" s="69">
+        <f t="shared" si="4"/>
+        <v>3.4722222222222219E-7</v>
+      </c>
+      <c r="J6" s="70">
+        <f t="shared" si="5"/>
+        <v>446.68359215096331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="70">
+        <v>2369</v>
+      </c>
+      <c r="C7" s="52">
+        <v>58</v>
+      </c>
+      <c r="D7" s="52">
+        <v>22647</v>
+      </c>
+      <c r="E7" s="68">
+        <f t="shared" si="1"/>
+        <v>3.3745650607227651</v>
+      </c>
+      <c r="F7" s="68">
+        <f t="shared" si="2"/>
+        <v>1.7634279935629373</v>
+      </c>
+      <c r="G7" s="68">
+        <f t="shared" si="3"/>
+        <v>4.3550106800911461</v>
+      </c>
+      <c r="H7" s="69">
+        <f t="shared" si="4"/>
+        <v>6.7129629629629619E-7</v>
+      </c>
+      <c r="J7" s="70">
+        <f t="shared" si="5"/>
+        <v>1412.5375446227545</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="70">
+        <v>10224</v>
+      </c>
+      <c r="C8" s="52">
+        <v>132</v>
+      </c>
+      <c r="D8" s="52">
+        <v>95076</v>
+      </c>
+      <c r="E8" s="68">
+        <f t="shared" si="1"/>
+        <v>4.0096208408143248</v>
+      </c>
+      <c r="F8" s="68">
+        <f t="shared" si="2"/>
+        <v>2.12057393120585</v>
+      </c>
+      <c r="G8" s="68">
+        <f t="shared" si="3"/>
+        <v>4.9780709019742115</v>
+      </c>
+      <c r="H8" s="69">
+        <f t="shared" si="4"/>
+        <v>1.5277777777777776E-6</v>
+      </c>
+      <c r="J8" s="70">
+        <f t="shared" si="5"/>
+        <v>4466.8359215096343</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="70">
+        <v>40468</v>
+      </c>
+      <c r="C9" s="52">
+        <v>507</v>
+      </c>
+      <c r="D9" s="52">
+        <v>376308</v>
+      </c>
+      <c r="E9" s="68">
+        <f t="shared" si="1"/>
+        <v>4.6071117413219582</v>
+      </c>
+      <c r="F9" s="68">
+        <f t="shared" si="2"/>
+        <v>2.705007959333336</v>
+      </c>
+      <c r="G9" s="68">
+        <f t="shared" si="3"/>
+        <v>5.5755434511631385</v>
+      </c>
+      <c r="H9" s="69">
+        <f t="shared" si="4"/>
+        <v>5.8680555555555558E-6</v>
+      </c>
+      <c r="J9" s="70">
+        <f t="shared" si="5"/>
+        <v>14125.375446227561</v>
+      </c>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="70">
+        <v>145640</v>
+      </c>
+      <c r="C10" s="52">
+        <v>2073</v>
+      </c>
+      <c r="D10" s="52">
+        <v>1361092</v>
+      </c>
+      <c r="E10" s="68">
+        <f t="shared" si="1"/>
+        <v>5.1632806702619058</v>
+      </c>
+      <c r="F10" s="68">
+        <f t="shared" si="2"/>
+        <v>3.3165993020938607</v>
+      </c>
+      <c r="G10" s="68">
+        <f t="shared" si="3"/>
+        <v>6.1338874813693645</v>
+      </c>
+      <c r="H10" s="69">
+        <f t="shared" si="4"/>
+        <v>2.3993055555555557E-5</v>
+      </c>
+      <c r="J10" s="70">
+        <f t="shared" si="5"/>
+        <v>44668.359215096389</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="70">
+        <v>472073</v>
+      </c>
+      <c r="C11" s="52">
+        <v>6815</v>
+      </c>
+      <c r="D11" s="52">
+        <v>4432459</v>
+      </c>
+      <c r="E11" s="68">
+        <f t="shared" si="1"/>
+        <v>5.6740091618666817</v>
+      </c>
+      <c r="F11" s="68">
+        <f t="shared" si="2"/>
+        <v>3.8334658601706924</v>
+      </c>
+      <c r="G11" s="68">
+        <f t="shared" si="3"/>
+        <v>6.6466447270916555</v>
+      </c>
+      <c r="H11" s="69">
+        <f t="shared" si="4"/>
+        <v>7.8877314814814798E-5</v>
+      </c>
+      <c r="J11" s="70">
+        <f t="shared" si="5"/>
+        <v>141253.75446227577</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="70">
+        <v>1362899</v>
+      </c>
+      <c r="C12" s="52">
+        <v>22364</v>
+      </c>
+      <c r="D12" s="52">
+        <v>12807567</v>
+      </c>
+      <c r="E12" s="68">
+        <f t="shared" si="1"/>
+        <v>6.1344636728794777</v>
+      </c>
+      <c r="F12" s="68">
+        <f t="shared" si="2"/>
+        <v>4.3495494835866353</v>
+      </c>
+      <c r="G12" s="68">
+        <f t="shared" si="3"/>
+        <v>7.1074666364714068</v>
+      </c>
+      <c r="H12" s="69">
+        <f t="shared" si="4"/>
+        <v>2.5884259259259263E-4</v>
+      </c>
+      <c r="J12" s="70">
+        <f t="shared" si="5"/>
+        <v>446683.59215096442</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="70">
+        <v>3471361</v>
+      </c>
+      <c r="C13" s="52">
+        <v>59927</v>
+      </c>
+      <c r="D13" s="52">
+        <v>32603225</v>
+      </c>
+      <c r="E13" s="68">
+        <f t="shared" si="1"/>
+        <v>6.5404997799507534</v>
+      </c>
+      <c r="F13" s="68">
+        <f t="shared" si="2"/>
+        <v>4.7776225370647989</v>
+      </c>
+      <c r="G13" s="68">
+        <f t="shared" si="3"/>
+        <v>7.5132605611240919</v>
+      </c>
+      <c r="H13" s="69">
+        <f t="shared" si="4"/>
+        <v>6.9359953703703717E-4</v>
+      </c>
+      <c r="J13" s="70">
+        <f t="shared" si="5"/>
+        <v>1412537.5446227565</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="70">
+        <v>7730168</v>
+      </c>
+      <c r="C14" s="52">
+        <v>157089</v>
+      </c>
+      <c r="D14" s="52">
+        <v>72684473</v>
+      </c>
+      <c r="E14" s="68">
+        <f t="shared" si="1"/>
+        <v>6.8881889325574086</v>
+      </c>
+      <c r="F14" s="68">
+        <f t="shared" si="2"/>
+        <v>5.19614577506825</v>
+      </c>
+      <c r="G14" s="68">
+        <f t="shared" si="3"/>
+        <v>7.861441645926071</v>
+      </c>
+      <c r="H14" s="69">
+        <f t="shared" si="4"/>
+        <v>1.8181597222222223E-3</v>
+      </c>
+      <c r="J14" s="70">
+        <f t="shared" si="5"/>
+        <v>4466835.9215096412</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="70">
+        <v>14908890</v>
+      </c>
+      <c r="C15" s="52">
+        <v>298718</v>
+      </c>
+      <c r="D15" s="52">
+        <v>140455916</v>
+      </c>
+      <c r="E15" s="68">
+        <f t="shared" si="1"/>
+        <v>7.1734453104670832</v>
+      </c>
+      <c r="F15" s="68">
+        <f t="shared" si="2"/>
+        <v>5.4752613928925244</v>
+      </c>
+      <c r="G15" s="68">
+        <f t="shared" si="3"/>
+        <v>8.1475400363965864</v>
+      </c>
+      <c r="H15" s="69">
+        <f t="shared" si="4"/>
+        <v>3.457384259259259E-3</v>
+      </c>
+      <c r="J15" s="70">
+        <f t="shared" si="5"/>
+        <v>14125375.446227582</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="70">
+        <v>24704588</v>
+      </c>
+      <c r="C16" s="52">
+        <v>535790</v>
+      </c>
+      <c r="D16" s="52">
+        <v>233554264</v>
+      </c>
+      <c r="E16" s="68">
+        <f t="shared" si="1"/>
+        <v>7.3927776155288747</v>
+      </c>
+      <c r="F16" s="68">
+        <f t="shared" si="2"/>
+        <v>5.7289946036631063</v>
+      </c>
+      <c r="G16" s="68">
+        <f t="shared" si="3"/>
+        <v>8.3683878006101704</v>
+      </c>
+      <c r="H16" s="69">
+        <f t="shared" si="4"/>
+        <v>6.2012731481481476E-3</v>
+      </c>
+      <c r="J16" s="70">
+        <f t="shared" si="5"/>
+        <v>44668359.215096377</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>